<commit_message>
Small adjustments so that post processig functions now work with the new output files which include additional columns for sensitivity.
</commit_message>
<xml_diff>
--- a/ccs_2DOC_CAMELS.xlsx
+++ b/ccs_2DOC_CAMELS.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmoffice-my.sharepoint.com/personal/rvanderh_uvm_edu/Documents/Documents/_UVM/Research/CIROH/TEVA/Holoviews/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmoffice-my.sharepoint.com/personal/rvanderh_uvm_edu/Documents/Documents/_UVM/Research/CIROH/TEVA/TEVA_Post_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="11_15C3EFF545E4183B4D183195395BDA1666CEA85E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B46B568E-351C-A84C-A4BE-B56752F16B24}"/>
@@ -1317,10 +1317,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6005,7 +6001,7 @@
   <dimension ref="A1:BR97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:BR1"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>